<commit_message>
fixed xls diff error
</commit_message>
<xml_diff>
--- a/unitycar.xlsx
+++ b/unitycar.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Aerodynamics" sheetId="5" r:id="rId1"/>
@@ -763,7 +763,7 @@
           <c:x val="0.10716885389326336"/>
           <c:y val="6.7179700774178966E-2"/>
           <c:w val="0.79354179819806969"/>
-          <c:h val="0.81684047680438199"/>
+          <c:h val="0.81684047680438221"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -817,8 +817,8 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="178782208"/>
-        <c:axId val="178784512"/>
+        <c:axId val="169429248"/>
+        <c:axId val="169452288"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -871,11 +871,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="178804992"/>
-        <c:axId val="178803072"/>
+        <c:axId val="169472768"/>
+        <c:axId val="169454208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="178782208"/>
+        <c:axId val="169429248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -896,16 +896,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="178784512"/>
+        <c:crossAx val="169452288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="178784512"/>
+        <c:axId val="169452288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -926,16 +925,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="178782208"/>
+        <c:crossAx val="169429248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="178803072"/>
+        <c:axId val="169454208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -956,16 +954,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="178804992"/>
+        <c:crossAx val="169472768"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="178804992"/>
+        <c:axId val="169472768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -973,7 +970,7 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="178803072"/>
+        <c:crossAx val="169454208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -984,9 +981,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.13991256387959103"/>
-          <c:y val="0.29817489438505473"/>
-          <c:w val="0.11925365607665189"/>
+          <c:x val="0.13991256387959106"/>
+          <c:y val="0.2981748943850549"/>
+          <c:w val="0.11925365607665192"/>
           <c:h val="0.12146373390983572"/>
         </c:manualLayout>
       </c:layout>
@@ -995,7 +992,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1038,7 +1035,7 @@
           <c:x val="0.10716885389326336"/>
           <c:y val="0.13564967840558387"/>
           <c:w val="0.7759889487498276"/>
-          <c:h val="0.74837039600819355"/>
+          <c:h val="0.74837039600819377"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1227,8 +1224,8 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="186463744"/>
-        <c:axId val="186466304"/>
+        <c:axId val="185266176"/>
+        <c:axId val="185268480"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1437,11 +1434,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="186482688"/>
-        <c:axId val="186468224"/>
+        <c:axId val="176691456"/>
+        <c:axId val="176689536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="186463744"/>
+        <c:axId val="185266176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -1468,20 +1465,20 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.45785918865405045"/>
+              <c:x val="0.45785918865405051"/>
               <c:y val="0.91133685212425353"/>
             </c:manualLayout>
           </c:layout>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186466304"/>
+        <c:crossAx val="185268480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="186466304"/>
+        <c:axId val="185268480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1507,12 +1504,12 @@
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186463744"/>
+        <c:crossAx val="185266176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="186468224"/>
+        <c:axId val="176689536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1537,12 +1534,12 @@
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186482688"/>
+        <c:crossAx val="176691456"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="186482688"/>
+        <c:axId val="176691456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1550,7 +1547,7 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="186468224"/>
+        <c:crossAx val="176689536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1562,9 +1559,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.59924851498825749"/>
-          <c:y val="0.47489083095382362"/>
+          <c:y val="0.47489083095382367"/>
           <c:w val="0.18457409325075061"/>
-          <c:h val="0.18618186240233511"/>
+          <c:h val="0.18618186240233514"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -1572,7 +1569,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1607,8 +1604,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.9002187226596826E-2"/>
-          <c:y val="0.11200668098305909"/>
+          <c:x val="7.9002187226596854E-2"/>
+          <c:y val="0.11200668098305912"/>
           <c:w val="0.8896019980223826"/>
           <c:h val="0.77201360057265567"/>
         </c:manualLayout>
@@ -1681,16 +1678,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.18</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3599999999999999</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.48</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.6</c:v>
@@ -1780,16 +1777,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.88</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.82</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.64</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.52</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.4</c:v>
@@ -1813,11 +1810,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="186253696"/>
-        <c:axId val="186255616"/>
+        <c:axId val="176700032"/>
+        <c:axId val="176730880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="186253696"/>
+        <c:axId val="176700032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1843,13 +1840,13 @@
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186255616"/>
+        <c:crossAx val="176730880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="186255616"/>
+        <c:axId val="176730880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1875,7 +1872,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186253696"/>
+        <c:crossAx val="176700032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1889,7 +1886,7 @@
           <c:x val="9.5833039198358963E-2"/>
           <c:y val="0.10618181818181818"/>
           <c:w val="0.11949282714293009"/>
-          <c:h val="0.10959341445955628"/>
+          <c:h val="0.1095934144595563"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -1897,7 +1894,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1928,7 +1925,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout>
@@ -1936,7 +1932,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.118383334994518"/>
+          <c:x val="0.11838333499451799"/>
           <c:y val="0.19480351414406533"/>
           <c:w val="0.82229708628193632"/>
           <c:h val="0.68921660834062359"/>
@@ -2005,11 +2001,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="186272384"/>
-        <c:axId val="186290944"/>
+        <c:axId val="185336960"/>
+        <c:axId val="185338880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="186272384"/>
+        <c:axId val="185336960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2031,16 +2027,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186290944"/>
+        <c:crossAx val="185338880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="186290944"/>
+        <c:axId val="185338880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2062,11 +2057,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186272384"/>
+        <c:crossAx val="185336960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2075,7 +2069,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2101,7 +2095,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2168,11 +2161,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="187646336"/>
-        <c:axId val="187648256"/>
+        <c:axId val="185371264"/>
+        <c:axId val="185381632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="187646336"/>
+        <c:axId val="185371264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.6"/>
@@ -2194,16 +2187,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="187648256"/>
+        <c:crossAx val="185381632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="187648256"/>
+        <c:axId val="185381632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2229,14 +2221,14 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="1.3888888888888911E-2"/>
-              <c:y val="0.29846274424030361"/>
+              <c:x val="1.3888888888888914E-2"/>
+              <c:y val="0.29846274424030367"/>
             </c:manualLayout>
           </c:layout>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="187646336"/>
+        <c:crossAx val="185371264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
@@ -2246,7 +2238,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2704,7 +2696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3877,7 +3869,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -4932,7 +4926,7 @@
         <v>0</v>
       </c>
       <c r="F63" s="3">
-        <f xml:space="preserve"> E63 * $B$60</f>
+        <f xml:space="preserve"> IF(ABS(E63) &gt; ABS($B$60), $B$60 * SIGN(E63), E63)</f>
         <v>0</v>
       </c>
       <c r="G63" s="3">
@@ -4960,44 +4954,44 @@
         <v>-0.2</v>
       </c>
       <c r="F64" s="3">
-        <f t="shared" ref="F64:F73" si="9" xml:space="preserve"> E64 * $B$60</f>
-        <v>-0.12</v>
+        <f t="shared" ref="F64:F73" si="9" xml:space="preserve"> IF(ABS(E64) &gt; ABS($B$60), $B$60 * SIGN(E64), E64)</f>
+        <v>-0.2</v>
       </c>
       <c r="G64" s="3">
         <f t="shared" ref="G64:G73" si="10" xml:space="preserve"> 1 - F64</f>
-        <v>1.1200000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="H64" s="3">
         <f t="shared" ref="H64:H73" si="11">1 + F64</f>
-        <v>0.88</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="65" spans="2:8">
       <c r="B65" s="14">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="C65" s="14">
         <v>0.2</v>
       </c>
       <c r="D65" s="6">
         <f t="shared" si="7"/>
-        <v>0.15000000000000002</v>
+        <v>0.2</v>
       </c>
       <c r="E65" s="3">
         <f t="shared" si="8"/>
-        <v>-0.30000000000000004</v>
+        <v>-0.4</v>
       </c>
       <c r="F65" s="3">
         <f t="shared" si="9"/>
-        <v>-0.18000000000000002</v>
+        <v>-0.4</v>
       </c>
       <c r="G65" s="3">
         <f t="shared" si="10"/>
-        <v>1.18</v>
+        <v>1.4</v>
       </c>
       <c r="H65" s="3">
         <f t="shared" si="11"/>
-        <v>0.82</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="66" spans="2:8">
@@ -5017,15 +5011,15 @@
       </c>
       <c r="F66" s="3">
         <f t="shared" si="9"/>
-        <v>-0.36</v>
+        <v>-0.6</v>
       </c>
       <c r="G66" s="3">
         <f t="shared" si="10"/>
-        <v>1.3599999999999999</v>
+        <v>1.6</v>
       </c>
       <c r="H66" s="3">
         <f t="shared" si="11"/>
-        <v>0.64</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="67" spans="2:8">
@@ -5045,15 +5039,15 @@
       </c>
       <c r="F67" s="3">
         <f t="shared" si="9"/>
-        <v>-0.48</v>
+        <v>-0.6</v>
       </c>
       <c r="G67" s="3">
         <f t="shared" si="10"/>
-        <v>1.48</v>
+        <v>1.6</v>
       </c>
       <c r="H67" s="3">
         <f t="shared" si="11"/>
-        <v>0.52</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="68" spans="2:8">

</xml_diff>